<commit_message>
data added and network function change to 10 node
</commit_message>
<xml_diff>
--- a/flavour_foodname.xlsx
+++ b/flavour_foodname.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>food_flavour</t>
   </si>
@@ -51,84 +51,153 @@
     <t>Banan, rå</t>
   </si>
   <si>
-    <t>Delta-Cadinene \nHerbal &amp; woody</t>
-  </si>
-  <si>
-    <t>Neomenthol \nMinty &amp; Sweet</t>
-  </si>
-  <si>
-    <t>Epicatechin \nBitter</t>
-  </si>
-  <si>
-    <t>(Z)-Cinnamyl Alcohol \nCinnamic &amp; Spicy</t>
-  </si>
-  <si>
-    <t>1-Dodecanol \nFatty &amp; Earthy</t>
-  </si>
-  <si>
-    <t>Apple \n172</t>
-  </si>
-  <si>
-    <t>Grape \n149</t>
-  </si>
-  <si>
-    <t>Strawberry \n149</t>
-  </si>
-  <si>
-    <t>Tea \n140</t>
-  </si>
-  <si>
-    <t>Jordbær, rå</t>
-  </si>
-  <si>
-    <t>Straberry \n206 Flavor Molecules</t>
+    <t>Delta-Cadinene
+ (Herbal &amp; Woody)</t>
   </si>
   <si>
     <t>Neomenthol
-Minty &amp; Sweet</t>
+(Minty &amp; Sweet)</t>
   </si>
   <si>
     <t>Epicatechin 
-Bitter</t>
+(Bitter)</t>
   </si>
   <si>
     <t>(Z)-Cinnamyl Alcohol
-Cinnamic &amp; Spicy</t>
+(Cinnamic &amp; Spicy)</t>
   </si>
   <si>
     <t>1-Dodecanol
-Fatty &amp; Earthy</t>
+(Fatty &amp; Earthy)</t>
+  </si>
+  <si>
+    <t>Banana
+(206 flavor 
+molecules)</t>
+  </si>
+  <si>
+    <t>Grape
+ (149 flavor
+molecules)</t>
   </si>
   <si>
     <t>Apple
-172 molecules</t>
+(172 flavor
+molecules)</t>
   </si>
   <si>
     <t>Strawberry
-149 molecules</t>
+(149 flavor
+molecules)</t>
   </si>
   <si>
     <t>Tea
-140 molecules</t>
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Pineapple
+(220 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Ananas, rå</t>
+  </si>
+  <si>
+    <t>item_pair5</t>
+  </si>
+  <si>
+    <t>item_pair6</t>
+  </si>
+  <si>
+    <t>item_pair7</t>
+  </si>
+  <si>
+    <t>item_pair8</t>
+  </si>
+  <si>
+    <t>item_pair9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apple
+(168 flavor
+molecules)
+</t>
+  </si>
+  <si>
+    <t>Strawberry
+(159 flavor
+molecules)</t>
   </si>
   <si>
     <t>Grape
- 149 molecules</t>
-  </si>
-  <si>
-    <t>Banana
-206 Flavor molecules</t>
-  </si>
-  <si>
-    <t>Delta-Cadinene
- Herbal &amp; Woody</t>
+(146 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Cocoa
+(146 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Mango
+(145 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Tea
+(145 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Passionfruit (142 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Papaya
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Peach
+(139 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Alpha-Terpineol
+(Mint &amp; Citrus)</t>
+  </si>
+  <si>
+    <t>passionfruit
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Papaya
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Guava
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Melon
+(140 flavor
+molecules)</t>
+  </si>
+  <si>
+    <t>Apricot
+(140 flavor
+molecules)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +231,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,23 +273,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,27 +609,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
     <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
+      <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -540,76 +667,357 @@
       <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="30">
+      <c r="L1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="60">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="75">
+      <c r="A3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="K3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
+      <c r="L3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="4"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="4"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="4"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="4"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="4"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="4"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
network function adjusted for 10-10 nodes
</commit_message>
<xml_diff>
--- a/flavour_foodname.xlsx
+++ b/flavour_foodname.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>food_flavour</t>
   </si>
@@ -191,6 +191,18 @@
     <t>Apricot
 (140 flavor
 molecules)</t>
+  </si>
+  <si>
+    <t>flavour_6</t>
+  </si>
+  <si>
+    <t>flavour_7</t>
+  </si>
+  <si>
+    <t>flavour_8</t>
+  </si>
+  <si>
+    <t>flavour_9</t>
   </si>
 </sst>
 </file>
@@ -609,33 +621,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="11" width="24" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -656,34 +669,46 @@
         <v>5</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="60">
+    <row r="2" spans="1:20" ht="60">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -706,34 +731,46 @@
         <v>15</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="Q2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="S2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="75">
+    <row r="3" spans="1:20" ht="60">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
@@ -755,35 +792,47 @@
       <c r="G3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:20">
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -794,8 +843,12 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -806,8 +859,12 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -818,8 +875,12 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -830,8 +891,12 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -842,8 +907,12 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -854,8 +923,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -866,8 +939,12 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -878,8 +955,12 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -890,8 +971,12 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -902,8 +987,12 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="4"/>
       <c r="B14" s="9"/>
       <c r="C14" s="4"/>
@@ -915,8 +1004,12 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="4"/>
       <c r="B15" s="9"/>
       <c r="C15" s="4"/>
@@ -928,8 +1021,12 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="4"/>
       <c r="B16" s="9"/>
       <c r="C16" s="4"/>
@@ -941,8 +1038,12 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="4"/>
       <c r="B17" s="9"/>
       <c r="C17" s="4"/>
@@ -954,8 +1055,12 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="4"/>
       <c r="B18" s="9"/>
       <c r="C18" s="4"/>
@@ -967,8 +1072,12 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="4"/>
       <c r="B19" s="9"/>
       <c r="C19" s="4"/>
@@ -980,8 +1089,12 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="4"/>
       <c r="B20" s="9"/>
       <c r="C20" s="4"/>
@@ -993,8 +1106,12 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="4"/>
       <c r="B21" s="9"/>
       <c r="C21" s="4"/>
@@ -1006,17 +1123,21 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:15">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:15">
       <c r="A26" s="3"/>
     </row>
   </sheetData>

</xml_diff>